<commit_message>
New Testcases: Div Address, Terms Code and Scrap Reason Code
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/CRUD-Inventory Location ID.xlsx
+++ b/templates/AutomationOrg/CRUD-Inventory Location ID.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkakade\Provar\Workspace\System Setup\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C9FA54-A081-4C99-B65C-92726953CCB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359632AB-3949-4BF3-ABCE-4231505DF245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1428" yWindow="3024" windowWidth="15912" windowHeight="8964" xr2:uid="{BE6563E9-F1E6-4FD9-B827-A5B609B0DDA1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Site</t>
   </si>
@@ -69,6 +69,36 @@
   </si>
   <si>
     <t>PK Loc ID - OH</t>
+  </si>
+  <si>
+    <t>Backflush Location</t>
+  </si>
+  <si>
+    <t>Inspection Order Location</t>
+  </si>
+  <si>
+    <t>Vendor Location</t>
+  </si>
+  <si>
+    <t>Issue Sequence for Backflush</t>
+  </si>
+  <si>
+    <t>PK-N</t>
+  </si>
+  <si>
+    <t>Non-nettable</t>
+  </si>
+  <si>
+    <t>PK NN Loc ID</t>
+  </si>
+  <si>
+    <t>Consigned</t>
+  </si>
+  <si>
+    <t>PK Cn Loc ID</t>
+  </si>
+  <si>
+    <t>PK-C</t>
   </si>
 </sst>
 </file>
@@ -420,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26DB4FC8-49EA-488C-AC77-DD2C86B6C974}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,10 +464,13 @@
     <col min="4" max="4" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,8 +489,20 @@
       <c r="F1" t="s">
         <v>8</v>
       </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -474,6 +519,82 @@
         <v>1</v>
       </c>
       <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>1</v>
       </c>
     </row>
@@ -487,11 +608,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>